<commit_message>
Rename marching cubes to watershed
</commit_message>
<xml_diff>
--- a/results/ejection_fraction_comparison_results.xlsx
+++ b/results/ejection_fraction_comparison_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkkad\Desktop\github_repos\heart_cardiac_mri_image_processing\data_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkkad\Desktop\github_repos\heart_cardiac_mri_image_processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988EB5E6-A5E4-4C8F-AA58-EFD86EC38D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3022044E-AB35-482E-BB43-249DE4C29C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10164" yWindow="2400" windowWidth="11124" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>Std Error</t>
   </si>
   <si>
-    <t>Marching Cubes</t>
+    <t>Edge Detection</t>
   </si>
   <si>
     <t>Heart failure with infarct</t>
@@ -61,10 +61,10 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Otsu</t>
+  </si>
+  <si>
     <t>Watershed</t>
-  </si>
-  <si>
-    <t>Edge Detection</t>
   </si>
 </sst>
 </file>
@@ -429,16 +429,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -469,10 +464,10 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>12.03768911223059</v>
+        <v>14.533595111867021</v>
       </c>
       <c r="E2">
-        <v>13.53116963868135</v>
+        <v>16.148542165749522</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -486,10 +481,10 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>195.98449100186849</v>
+        <v>102.7973195300453</v>
       </c>
       <c r="E3">
-        <v>16.23740465086442</v>
+        <v>99.284519657733725</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -503,10 +498,10 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>139.12969927417731</v>
+        <v>101.8230655722588</v>
       </c>
       <c r="E4">
-        <v>14.880036838303241</v>
+        <v>101.4611836238015</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -520,10 +515,10 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>15.110845585629679</v>
+        <v>16.813198102189322</v>
       </c>
       <c r="E5">
-        <v>16.791451045920741</v>
+        <v>20.0376588623262</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -537,10 +532,10 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>165.8681147955904</v>
+        <v>100.2943306115923</v>
       </c>
       <c r="E6">
-        <v>27.278996653032319</v>
+        <v>108.1059908672057</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -554,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>117.05796284591619</v>
+        <v>50.176953938103843</v>
       </c>
       <c r="E7">
-        <v>18.51043123435031</v>
+        <v>65.902816281114156</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -571,10 +566,10 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>19.655052036391329</v>
+        <v>13.84499381841573</v>
       </c>
       <c r="E8">
-        <v>20.12392812487505</v>
+        <v>16.212580140341039</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -588,10 +583,10 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>54.748522663978591</v>
+        <v>150.77097147398121</v>
       </c>
       <c r="E9">
-        <v>20.573987391585149</v>
+        <v>157.02951863135701</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -605,10 +600,10 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>13.90189030222141</v>
+        <v>62.187452474357329</v>
       </c>
       <c r="E10">
-        <v>12.89567834873691</v>
+        <v>82.478070129762301</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -622,10 +617,10 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>22.0318377319491</v>
+        <v>13.012877906533349</v>
       </c>
       <c r="E11">
-        <v>15.85739820227772</v>
+        <v>16.23338314328134</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -639,10 +634,10 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <v>44.987293088577673</v>
+        <v>101.59066637534571</v>
       </c>
       <c r="E12">
-        <v>23.73204003206974</v>
+        <v>72.585021128572961</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -656,10 +651,10 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>14.033924547349899</v>
+        <v>57.21813766268955</v>
       </c>
       <c r="E13">
-        <v>20.009258906245201</v>
+        <v>48.36376403274064</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -724,10 +719,10 @@
         <v>7</v>
       </c>
       <c r="D17">
-        <v>34.439532528504699</v>
+        <v>32.867396690934299</v>
       </c>
       <c r="E17">
-        <v>18.94421846101006</v>
+        <v>18.87231263031746</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -741,10 +736,10 @@
         <v>8</v>
       </c>
       <c r="D18">
-        <v>448.34060850217099</v>
+        <v>428.17025270436721</v>
       </c>
       <c r="E18">
-        <v>500.72980554424231</v>
+        <v>482.57526238321861</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -758,10 +753,10 @@
         <v>9</v>
       </c>
       <c r="D19">
-        <v>106.17206938067601</v>
+        <v>102.9561926671045</v>
       </c>
       <c r="E19">
-        <v>136.7910473975459</v>
+        <v>132.2540520011988</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -826,10 +821,10 @@
         <v>7</v>
       </c>
       <c r="D23">
-        <v>51.838164536490133</v>
+        <v>17.861086752801722</v>
       </c>
       <c r="E23">
-        <v>37.52774551523104</v>
+        <v>18.126721849355171</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -843,10 +838,10 @@
         <v>8</v>
       </c>
       <c r="D24">
-        <v>3389.3923043861842</v>
+        <v>293.86695966782639</v>
       </c>
       <c r="E24">
-        <v>1749.3923214978199</v>
+        <v>298.87144095546188</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -860,10 +855,10 @@
         <v>9</v>
       </c>
       <c r="D25">
-        <v>3188.5058362879281</v>
+        <v>56.02734316913179</v>
       </c>
       <c r="E25">
-        <v>2012.8366572065349</v>
+        <v>44.214879453982093</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -877,10 +872,10 @@
         <v>7</v>
       </c>
       <c r="D26">
-        <v>14.533595111867021</v>
+        <v>12.03768911223059</v>
       </c>
       <c r="E26">
-        <v>16.148542165749522</v>
+        <v>13.53116963868135</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -894,10 +889,10 @@
         <v>8</v>
       </c>
       <c r="D27">
-        <v>102.7973195300453</v>
+        <v>195.98449100186849</v>
       </c>
       <c r="E27">
-        <v>99.284519657733725</v>
+        <v>16.23740465086442</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -911,10 +906,10 @@
         <v>9</v>
       </c>
       <c r="D28">
-        <v>101.8230655722588</v>
+        <v>139.12969927417731</v>
       </c>
       <c r="E28">
-        <v>101.4611836238015</v>
+        <v>14.880036838303241</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -928,10 +923,10 @@
         <v>7</v>
       </c>
       <c r="D29">
-        <v>16.813198102189322</v>
+        <v>15.110845585629679</v>
       </c>
       <c r="E29">
-        <v>20.0376588623262</v>
+        <v>16.791451045920741</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -945,10 +940,10 @@
         <v>8</v>
       </c>
       <c r="D30">
-        <v>100.2943306115923</v>
+        <v>165.8681147955904</v>
       </c>
       <c r="E30">
-        <v>108.1059908672057</v>
+        <v>27.278996653032319</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -962,10 +957,10 @@
         <v>9</v>
       </c>
       <c r="D31">
-        <v>50.176953938103843</v>
+        <v>117.05796284591619</v>
       </c>
       <c r="E31">
-        <v>65.902816281114156</v>
+        <v>18.51043123435031</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -979,10 +974,10 @@
         <v>7</v>
       </c>
       <c r="D32">
-        <v>13.84499381841573</v>
+        <v>19.655052036391329</v>
       </c>
       <c r="E32">
-        <v>16.212580140341039</v>
+        <v>20.12392812487505</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -996,10 +991,10 @@
         <v>8</v>
       </c>
       <c r="D33">
-        <v>150.77097147398121</v>
+        <v>54.748522663978591</v>
       </c>
       <c r="E33">
-        <v>157.02951863135701</v>
+        <v>20.573987391585149</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1013,10 +1008,10 @@
         <v>9</v>
       </c>
       <c r="D34">
-        <v>62.187452474357329</v>
+        <v>13.90189030222141</v>
       </c>
       <c r="E34">
-        <v>82.478070129762301</v>
+        <v>12.89567834873691</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1030,10 +1025,10 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>13.012877906533349</v>
+        <v>22.0318377319491</v>
       </c>
       <c r="E35">
-        <v>16.23338314328134</v>
+        <v>15.85739820227772</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1047,10 +1042,10 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>101.59066637534571</v>
+        <v>44.987293088577673</v>
       </c>
       <c r="E36">
-        <v>72.585021128572961</v>
+        <v>23.73204003206974</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,10 +1059,10 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <v>57.21813766268955</v>
+        <v>14.033924547349899</v>
       </c>
       <c r="E37">
-        <v>48.36376403274064</v>
+        <v>20.009258906245201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>